<commit_message>
add: added new table
</commit_message>
<xml_diff>
--- a/data/wine_map/done/wine_test.xlsx
+++ b/data/wine_map/done/wine_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="120">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -52,6 +52,42 @@
     <t xml:space="preserve">precipitation</t>
   </si>
   <si>
+    <t xml:space="preserve">fixed_acidity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">volatile_acidity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">citric_acid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">residual_sugar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chlorides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free_sulfur_dioxide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total_sulfur_dioxide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sulphates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alcohol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">winecolor</t>
+  </si>
+  <si>
     <t xml:space="preserve">виноградник №1</t>
   </si>
   <si>
@@ -70,9 +106,60 @@
     <t xml:space="preserve">2022-12-01</t>
   </si>
   <si>
+    <t xml:space="preserve">0.27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">white</t>
+  </si>
+  <si>
     <t xml:space="preserve">2023-01-01</t>
   </si>
   <si>
+    <t xml:space="preserve">6.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Виноградник №2</t>
   </si>
   <si>
@@ -86,6 +173,213 @@
   </si>
   <si>
     <t xml:space="preserve">38.089649</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9951</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9956</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-02-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-04-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-08-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9961</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-06-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9953</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9964</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-03-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9972</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.1</t>
   </si>
 </sst>
 </file>
@@ -96,7 +390,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -117,11 +411,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -166,7 +455,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -175,7 +464,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -196,24 +489,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5:E5"/>
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6:V13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="16.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.15"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -243,26 +536,62 @@
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>10</v>
@@ -275,26 +604,62 @@
       </c>
       <c r="J2" s="0" t="n">
         <v>40</v>
+      </c>
+      <c r="K2" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q2" s="3" t="n">
+        <v>170</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>30</v>
@@ -307,26 +672,62 @@
       </c>
       <c r="J3" s="0" t="n">
         <v>11</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="3" t="n">
+        <v>132</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
+        <v>50</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>10</v>
@@ -339,26 +740,62 @@
       </c>
       <c r="J4" s="0" t="n">
         <v>40</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="3" t="n">
+        <v>97</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
+        <v>50</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>30</v>
@@ -371,6 +808,586 @@
       </c>
       <c r="J5" s="0" t="n">
         <v>11</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P5" s="3" t="n">
+        <v>47</v>
+      </c>
+      <c r="Q5" s="3" t="n">
+        <v>186</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="P6" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="3" t="n">
+        <v>121</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="P7" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="3" t="n">
+        <v>121</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="P8" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q8" s="3" t="n">
+        <v>96</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="P9" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q9" s="3" t="n">
+        <v>101</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="P10" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q10" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U10" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="P11" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="3" t="n">
+        <v>44</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P12" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q12" s="3" t="n">
+        <v>63</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="S12" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P13" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -378,8 +1395,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>